<commit_message>
Added Excel file with Nagupande and Lusulu flyround catches
</commit_message>
<xml_diff>
--- a/Data/Nagupande Flyround catches of G morsitans by month.xlsx
+++ b/Data/Nagupande Flyround catches of G morsitans by month.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>January</t>
   </si>
@@ -69,16 +69,19 @@
     <t>hunting]</t>
   </si>
   <si>
-    <t>Fly round</t>
-  </si>
-  <si>
-    <t>catch</t>
-  </si>
-  <si>
     <t>averages</t>
   </si>
   <si>
     <t>3-mnthly</t>
+  </si>
+  <si>
+    <t>Fly round catches</t>
+  </si>
+  <si>
+    <t>Nagupande</t>
+  </si>
+  <si>
+    <t>Lusulu</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -129,6 +132,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +151,1678 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.6292834578883741E-2"/>
+          <c:y val="1.7904040404040412E-2"/>
+          <c:w val="0.91689148350730965"/>
+          <c:h val="0.84384335480792194"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Nagupande</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Nagupande Fly round catches'!$Q$6:$Q$77</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>22647</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22678</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22706</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22737</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22767</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22798</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22828</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22859</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22890</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22920</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22951</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23043</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23071</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23102</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23132</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23163</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23193</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23224</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23255</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23285</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23316</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23346</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23377</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23408</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>23437</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23468</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23498</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>23529</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>23559</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23590</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>23621</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>23651</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>23682</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>23712</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>23743</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>23774</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>23802</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>23833</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>23863</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>23894</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>23924</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>23955</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>23986</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>24016</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>24047</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>24077</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>24108</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>24139</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>24167</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>24198</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>24228</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>24259</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>24289</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>24320</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>24351</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>24381</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>24412</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>24442</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>24473</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>24504</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>24532</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>24563</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>24593</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>24624</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>24654</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>24685</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>24716</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>24746</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>24777</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>24807</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Nagupande Fly round catches'!$T$6:$T$77</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>766</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>76.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>47.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>51.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43.3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>38.9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>47.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>23.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>32.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>24.4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>28.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>70.8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>37.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>50.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>30.8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>15.8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Lusulu</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Nagupande Fly round catches'!$U$6:$U$77</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>681</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>663</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>757</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>943</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>862</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>633</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>698</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>973</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>533</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>782</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1408</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1413</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1645</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1124</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1036</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>901</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1028</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>462</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>879</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1172</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1287</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>808</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>812</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>749</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1018</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1007</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>628</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>946</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>636</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>638</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>983</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>859</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>187</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="427871032"/>
+        <c:axId val="427870248"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="427871032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Month and year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45720515851549098"/>
+              <c:y val="0.94790593652248945"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427870248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="427870248"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Monthly catch (log scale)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="7.6288293161828041E-3"/>
+              <c:y val="0.29563693236975513"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427871032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.75899969807003187"/>
+          <c:y val="0.3866789946711206"/>
+          <c:w val="0.10855631357149059"/>
+          <c:h val="9.1967560133750403E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>10160</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,119 +2088,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:R82"/>
+  <dimension ref="B3:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AQ26" sqref="AQ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" style="1" customWidth="1"/>
-    <col min="3" max="17" width="6.6640625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="19" width="6.6640625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="R3" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="R4" s="6" t="s">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="T4" s="6"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="Q6" s="8">
+        <v>22647</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" s="2">
+        <v>306</v>
+      </c>
+      <c r="U6" s="2">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="Q7" s="8">
+        <v>22678</v>
+      </c>
+      <c r="R7" s="1">
+        <v>2</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="2">
+        <v>247</v>
+      </c>
+      <c r="U7" s="2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="O5" s="5"/>
-      <c r="P5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="P6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="2">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="P7" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R7" s="2">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" s="1">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>22706</v>
+      </c>
+      <c r="R8" s="1">
         <v>3</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R8" s="2">
+      <c r="T8" s="2">
         <v>477</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U8" s="2">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>22737</v>
+      </c>
+      <c r="R9" s="1">
         <v>4</v>
       </c>
-      <c r="R9" s="2">
+      <c r="T9" s="2">
         <v>492</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U9" s="2">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -534,14 +2245,20 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="P10" s="1">
+      <c r="Q10" s="8">
+        <v>22767</v>
+      </c>
+      <c r="R10" s="1">
         <v>5</v>
       </c>
-      <c r="R10" s="2">
+      <c r="T10" s="2">
         <v>304</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U10" s="2">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C11" s="4">
         <v>1962</v>
       </c>
@@ -566,14 +2283,20 @@
         <v>1967</v>
       </c>
       <c r="N11" s="4"/>
-      <c r="P11" s="1">
+      <c r="Q11" s="8">
+        <v>22798</v>
+      </c>
+      <c r="R11" s="1">
         <v>6</v>
       </c>
-      <c r="R11" s="2">
+      <c r="T11" s="2">
         <v>382</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U11" s="2">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,14 +2324,20 @@
         <v>1.9</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="P12" s="1">
+      <c r="Q12" s="8">
+        <v>22828</v>
+      </c>
+      <c r="R12" s="1">
         <v>7</v>
       </c>
-      <c r="R12" s="2">
+      <c r="T12" s="2">
         <v>297</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U12" s="2">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
@@ -654,14 +2383,20 @@
         <f>INT(AVERAGE(M12:M14)+0.5)</f>
         <v>4</v>
       </c>
-      <c r="P13" s="1">
+      <c r="Q13" s="8">
+        <v>22859</v>
+      </c>
+      <c r="R13" s="1">
         <v>8</v>
       </c>
-      <c r="R13" s="2">
+      <c r="T13" s="2">
         <v>627</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U13" s="2">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
@@ -689,14 +2424,20 @@
         <v>5</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="P14" s="1">
+      <c r="Q14" s="8">
+        <v>22890</v>
+      </c>
+      <c r="R14" s="1">
         <v>9</v>
       </c>
-      <c r="R14" s="2">
+      <c r="T14" s="2">
         <v>520</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U14" s="2">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -724,17 +2465,23 @@
         <v>6.1</v>
       </c>
       <c r="N15" s="2"/>
-      <c r="P15" s="1">
+      <c r="Q15" s="8">
+        <v>22920</v>
+      </c>
+      <c r="R15" s="1">
         <v>10</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="S15" s="1">
         <v>1</v>
       </c>
-      <c r="R15" s="2">
+      <c r="T15" s="2">
         <v>422</v>
       </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U15" s="2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -780,17 +2527,23 @@
         <f>INT(AVERAGE(M15:M17)+0.5)</f>
         <v>5</v>
       </c>
-      <c r="P16" s="1">
+      <c r="Q16" s="8">
+        <v>22951</v>
+      </c>
+      <c r="R16" s="1">
         <v>11</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="S16" s="1">
         <v>2</v>
       </c>
-      <c r="R16" s="2">
+      <c r="T16" s="2">
         <v>766</v>
       </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U16" s="2">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -818,17 +2571,23 @@
         <v>6.7</v>
       </c>
       <c r="N17" s="2"/>
-      <c r="P17" s="1">
+      <c r="Q17" s="8">
+        <v>22981</v>
+      </c>
+      <c r="R17" s="1">
         <v>12</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="S17" s="1">
         <v>3</v>
       </c>
-      <c r="R17" s="2">
+      <c r="T17" s="2">
         <v>1009</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U17" s="2">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -856,17 +2615,23 @@
         <v>1.4</v>
       </c>
       <c r="N18" s="2"/>
-      <c r="P18" s="1">
+      <c r="Q18" s="8">
+        <v>23012</v>
+      </c>
+      <c r="R18" s="1">
         <v>13</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="S18" s="1">
         <v>4</v>
       </c>
-      <c r="R18" s="2">
+      <c r="T18" s="2">
         <v>513</v>
       </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U18" s="2">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -912,17 +2677,23 @@
         <f>INT(AVERAGE(M18:M20)+0.5)</f>
         <v>3</v>
       </c>
-      <c r="P19" s="1">
+      <c r="Q19" s="8">
+        <v>23043</v>
+      </c>
+      <c r="R19" s="1">
         <v>14</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="S19" s="1">
         <v>5</v>
       </c>
-      <c r="R19" s="2">
+      <c r="T19" s="2">
         <v>580</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U19" s="2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
@@ -950,17 +2721,23 @@
         <v>3.9</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="P20" s="1">
+      <c r="Q20" s="8">
+        <v>23071</v>
+      </c>
+      <c r="R20" s="1">
         <v>15</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="S20" s="1">
         <v>6</v>
       </c>
-      <c r="R20" s="2">
+      <c r="T20" s="2">
         <v>342</v>
       </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U20" s="2">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
@@ -988,17 +2765,23 @@
         <v>1.4</v>
       </c>
       <c r="N21" s="2"/>
-      <c r="P21" s="1">
+      <c r="Q21" s="8">
+        <v>23102</v>
+      </c>
+      <c r="R21" s="1">
         <v>16</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="S21" s="1">
         <v>7</v>
       </c>
-      <c r="R21" s="2">
+      <c r="T21" s="2">
         <v>324</v>
       </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U21" s="2">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1044,17 +2827,23 @@
         <f>INT(AVERAGE(M21:M23)+0.5)</f>
         <v>2</v>
       </c>
-      <c r="P22" s="1">
+      <c r="Q22" s="8">
+        <v>23132</v>
+      </c>
+      <c r="R22" s="1">
         <v>17</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="S22" s="1">
         <v>8</v>
       </c>
-      <c r="R22" s="2">
+      <c r="T22" s="2">
         <v>211</v>
       </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U22" s="2">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1082,17 +2871,23 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N23" s="2"/>
-      <c r="P23" s="1">
+      <c r="Q23" s="8">
+        <v>23163</v>
+      </c>
+      <c r="R23" s="1">
         <v>18</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="S23" s="1">
         <v>9</v>
       </c>
-      <c r="R23" s="2">
+      <c r="T23" s="2">
         <v>118</v>
       </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U23" s="2">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1105,17 +2900,23 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="P24" s="1">
+      <c r="Q24" s="8">
+        <v>23193</v>
+      </c>
+      <c r="R24" s="1">
         <v>19</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="S24" s="1">
         <v>10</v>
       </c>
-      <c r="R24" s="2">
+      <c r="T24" s="2">
         <v>76.099999999999994</v>
       </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U24" s="2">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1125,17 +2926,23 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="P25" s="1">
+      <c r="Q25" s="8">
+        <v>23224</v>
+      </c>
+      <c r="R25" s="1">
         <v>20</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="S25" s="1">
         <v>11</v>
       </c>
-      <c r="R25" s="2">
+      <c r="T25" s="2">
         <v>95.6</v>
       </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U25" s="2">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,17 +2970,23 @@
         <v>576</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="P26" s="1">
+      <c r="Q26" s="8">
+        <v>23255</v>
+      </c>
+      <c r="R26" s="1">
         <v>21</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="S26" s="1">
         <v>12</v>
       </c>
-      <c r="R26" s="2">
+      <c r="T26" s="2">
         <v>47.8</v>
       </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U26" s="2">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1219,17 +3032,23 @@
         <f>INT(AVERAGE(M26:M28)+0.5)</f>
         <v>617</v>
       </c>
-      <c r="P27" s="1">
+      <c r="Q27" s="8">
+        <v>23285</v>
+      </c>
+      <c r="R27" s="1">
         <v>22</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="S27" s="1">
         <v>13</v>
       </c>
-      <c r="R27" s="2">
+      <c r="T27" s="2">
         <v>43.3</v>
       </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U27" s="2">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>2</v>
       </c>
@@ -1257,17 +3076,23 @@
         <v>638</v>
       </c>
       <c r="N28" s="2"/>
-      <c r="P28" s="1">
+      <c r="Q28" s="8">
+        <v>23316</v>
+      </c>
+      <c r="R28" s="1">
         <v>23</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="S28" s="1">
         <v>14</v>
       </c>
-      <c r="R28" s="2">
+      <c r="T28" s="2">
         <v>51.7</v>
       </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U28" s="2">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
@@ -1295,17 +3120,23 @@
         <v>529</v>
       </c>
       <c r="N29" s="2"/>
-      <c r="P29" s="1">
+      <c r="Q29" s="8">
+        <v>23346</v>
+      </c>
+      <c r="R29" s="1">
         <v>24</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="S29" s="1">
         <v>15</v>
       </c>
-      <c r="R29" s="2">
+      <c r="T29" s="2">
         <v>48.3</v>
       </c>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U29" s="2">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1351,17 +3182,23 @@
         <f>INT(AVERAGE(M29:M31)+0.5)</f>
         <v>695</v>
       </c>
-      <c r="P30" s="1">
+      <c r="Q30" s="8">
+        <v>23377</v>
+      </c>
+      <c r="R30" s="1">
         <v>25</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="S30" s="1">
         <v>16</v>
       </c>
-      <c r="R30" s="2">
+      <c r="T30" s="2">
         <v>43.3</v>
       </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U30" s="2">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
@@ -1389,17 +3226,23 @@
         <v>585</v>
       </c>
       <c r="N31" s="2"/>
-      <c r="P31" s="1">
+      <c r="Q31" s="8">
+        <v>23408</v>
+      </c>
+      <c r="R31" s="1">
         <v>26</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="S31" s="1">
         <v>17</v>
       </c>
-      <c r="R31" s="2">
+      <c r="T31" s="2">
         <v>38.9</v>
       </c>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U31" s="2">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
@@ -1427,17 +3270,23 @@
         <v>983</v>
       </c>
       <c r="N32" s="2"/>
-      <c r="P32" s="1">
+      <c r="Q32" s="8">
+        <v>23437</v>
+      </c>
+      <c r="R32" s="1">
         <v>27</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="S32" s="1">
         <v>18</v>
       </c>
-      <c r="R32" s="2">
+      <c r="T32" s="2">
         <v>28.9</v>
       </c>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U32" s="2">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1483,17 +3332,23 @@
         <f>INT(AVERAGE(M32:M34)+0.5)</f>
         <v>824</v>
       </c>
-      <c r="P33" s="1">
+      <c r="Q33" s="8">
+        <v>23468</v>
+      </c>
+      <c r="R33" s="1">
         <v>28</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="S33" s="1">
         <v>19</v>
       </c>
-      <c r="R33" s="2">
+      <c r="T33" s="2">
         <v>41.7</v>
       </c>
-    </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U33" s="2">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>8</v>
       </c>
@@ -1521,17 +3376,23 @@
         <v>630</v>
       </c>
       <c r="N34" s="2"/>
-      <c r="P34" s="1">
+      <c r="Q34" s="8">
+        <v>23498</v>
+      </c>
+      <c r="R34" s="1">
         <v>29</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="S34" s="1">
         <v>20</v>
       </c>
-      <c r="R34" s="2">
+      <c r="T34" s="2">
         <v>47.2</v>
       </c>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U34" s="2">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
@@ -1559,17 +3420,23 @@
         <v>336</v>
       </c>
       <c r="N35" s="2"/>
-      <c r="P35" s="1">
+      <c r="Q35" s="8">
+        <v>23529</v>
+      </c>
+      <c r="R35" s="1">
         <v>30</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="S35" s="1">
         <v>21</v>
       </c>
-      <c r="R35" s="2">
+      <c r="T35" s="2">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U35" s="2">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>10</v>
       </c>
@@ -1615,17 +3482,23 @@
         <f>INT(AVERAGE(M35:M37)+0.5)</f>
         <v>313</v>
       </c>
-      <c r="P36" s="1">
+      <c r="Q36" s="8">
+        <v>23559</v>
+      </c>
+      <c r="R36" s="1">
         <v>31</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="S36" s="1">
         <v>22</v>
       </c>
-      <c r="R36" s="2">
+      <c r="T36" s="2">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U36" s="2">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>11</v>
       </c>
@@ -1653,17 +3526,23 @@
         <v>187</v>
       </c>
       <c r="N37" s="2"/>
-      <c r="P37" s="1">
+      <c r="Q37" s="8">
+        <v>23590</v>
+      </c>
+      <c r="R37" s="1">
         <v>32</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="S37" s="1">
         <v>23</v>
       </c>
-      <c r="R37" s="2">
+      <c r="T37" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U37" s="2">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -1673,17 +3552,23 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
-      <c r="P38" s="1">
+      <c r="Q38" s="8">
+        <v>23621</v>
+      </c>
+      <c r="R38" s="1">
         <v>33</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="S38" s="1">
         <v>24</v>
       </c>
-      <c r="R38" s="2">
+      <c r="T38" s="2">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U38" s="2">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -1693,17 +3578,23 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
-      <c r="P39" s="1">
+      <c r="Q39" s="8">
+        <v>23651</v>
+      </c>
+      <c r="R39" s="1">
         <v>34</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="S39" s="1">
         <v>25</v>
       </c>
-      <c r="R39" s="2">
+      <c r="T39" s="2">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U39" s="2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1713,17 +3604,23 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
-      <c r="P40" s="1">
+      <c r="Q40" s="8">
+        <v>23682</v>
+      </c>
+      <c r="R40" s="1">
         <v>35</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="S40" s="1">
         <v>26</v>
       </c>
-      <c r="R40" s="2">
+      <c r="T40" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U40" s="2">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -1733,17 +3630,23 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
-      <c r="P41" s="1">
+      <c r="Q41" s="8">
+        <v>23712</v>
+      </c>
+      <c r="R41" s="1">
         <v>36</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="S41" s="1">
         <v>27</v>
       </c>
-      <c r="R41" s="2">
+      <c r="T41" s="2">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U41" s="2">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -1753,17 +3656,23 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
-      <c r="P42" s="1">
+      <c r="Q42" s="8">
+        <v>23743</v>
+      </c>
+      <c r="R42" s="1">
         <v>37</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="S42" s="1">
         <v>28</v>
       </c>
-      <c r="R42" s="2">
+      <c r="T42" s="2">
         <v>32.799999999999997</v>
       </c>
-    </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U42" s="2">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -1773,17 +3682,23 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
-      <c r="P43" s="1">
+      <c r="Q43" s="8">
+        <v>23774</v>
+      </c>
+      <c r="R43" s="1">
         <v>38</v>
       </c>
-      <c r="Q43" s="1">
+      <c r="S43" s="1">
         <v>29</v>
       </c>
-      <c r="R43" s="2">
+      <c r="T43" s="2">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U43" s="2">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -1793,17 +3708,23 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
-      <c r="P44" s="1">
+      <c r="Q44" s="8">
+        <v>23802</v>
+      </c>
+      <c r="R44" s="1">
         <v>39</v>
       </c>
-      <c r="Q44" s="1">
+      <c r="S44" s="1">
         <v>30</v>
       </c>
-      <c r="R44" s="2">
+      <c r="T44" s="2">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U44" s="2">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -1813,17 +3734,23 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
-      <c r="P45" s="1">
+      <c r="Q45" s="8">
+        <v>23833</v>
+      </c>
+      <c r="R45" s="1">
         <v>40</v>
       </c>
-      <c r="Q45" s="1">
+      <c r="S45" s="1">
         <v>31</v>
       </c>
-      <c r="R45" s="2">
+      <c r="T45" s="2">
         <v>28.9</v>
       </c>
-    </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U45" s="2">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -1833,17 +3760,23 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
-      <c r="P46" s="1">
+      <c r="Q46" s="8">
+        <v>23863</v>
+      </c>
+      <c r="R46" s="1">
         <v>41</v>
       </c>
-      <c r="Q46" s="1">
+      <c r="S46" s="1">
         <v>32</v>
       </c>
-      <c r="R46" s="2">
+      <c r="T46" s="2">
         <v>70.8</v>
       </c>
-    </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U46" s="2">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -1853,17 +3786,23 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
-      <c r="P47" s="1">
+      <c r="Q47" s="8">
+        <v>23894</v>
+      </c>
+      <c r="R47" s="1">
         <v>42</v>
       </c>
-      <c r="Q47" s="1">
+      <c r="S47" s="1">
         <v>33</v>
       </c>
-      <c r="R47" s="2">
+      <c r="T47" s="2">
         <v>37.799999999999997</v>
       </c>
-    </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U47" s="2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -1873,17 +3812,23 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
-      <c r="P48" s="1">
+      <c r="Q48" s="8">
+        <v>23924</v>
+      </c>
+      <c r="R48" s="1">
         <v>43</v>
       </c>
-      <c r="Q48" s="1">
+      <c r="S48" s="1">
         <v>34</v>
       </c>
-      <c r="R48" s="2">
+      <c r="T48" s="2">
         <v>23.6</v>
       </c>
-    </row>
-    <row r="49" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U48" s="2">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="49" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -1893,17 +3838,23 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
-      <c r="P49" s="1">
+      <c r="Q49" s="8">
+        <v>23955</v>
+      </c>
+      <c r="R49" s="1">
         <v>44</v>
       </c>
-      <c r="Q49" s="1">
+      <c r="S49" s="1">
         <v>35</v>
       </c>
-      <c r="R49" s="2">
+      <c r="T49" s="2">
         <v>50.3</v>
       </c>
-    </row>
-    <row r="50" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U49" s="2">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="50" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -1913,17 +3864,23 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
-      <c r="P50" s="1">
+      <c r="Q50" s="8">
+        <v>23986</v>
+      </c>
+      <c r="R50" s="1">
         <v>45</v>
       </c>
-      <c r="Q50" s="1">
+      <c r="S50" s="1">
         <v>36</v>
       </c>
-      <c r="R50" s="2">
+      <c r="T50" s="2">
         <v>30.8</v>
       </c>
-    </row>
-    <row r="51" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U50" s="2">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="51" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -1933,17 +3890,23 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
-      <c r="P51" s="1">
+      <c r="Q51" s="8">
+        <v>24016</v>
+      </c>
+      <c r="R51" s="1">
         <v>46</v>
       </c>
-      <c r="Q51" s="1">
+      <c r="S51" s="1">
         <v>37</v>
       </c>
-      <c r="R51" s="2">
+      <c r="T51" s="2">
         <v>22.2</v>
       </c>
-    </row>
-    <row r="52" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U51" s="2">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="52" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -1953,17 +3916,23 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
-      <c r="P52" s="1">
+      <c r="Q52" s="8">
+        <v>24047</v>
+      </c>
+      <c r="R52" s="1">
         <v>47</v>
       </c>
-      <c r="Q52" s="1">
+      <c r="S52" s="1">
         <v>38</v>
       </c>
-      <c r="R52" s="2">
+      <c r="T52" s="2">
         <v>26.9</v>
       </c>
-    </row>
-    <row r="53" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U52" s="2">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="53" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -1973,17 +3942,23 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
-      <c r="P53" s="1">
+      <c r="Q53" s="8">
+        <v>24077</v>
+      </c>
+      <c r="R53" s="1">
         <v>48</v>
       </c>
-      <c r="Q53" s="1">
+      <c r="S53" s="1">
         <v>39</v>
       </c>
-      <c r="R53" s="2">
+      <c r="T53" s="2">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="54" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U53" s="2">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="54" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -1993,17 +3968,23 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
-      <c r="P54" s="1">
+      <c r="Q54" s="8">
+        <v>24108</v>
+      </c>
+      <c r="R54" s="1">
         <v>49</v>
       </c>
-      <c r="Q54" s="1">
+      <c r="S54" s="1">
         <v>40</v>
       </c>
-      <c r="R54" s="2">
+      <c r="T54" s="2">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="55" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U54" s="2">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="55" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -2013,17 +3994,23 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
-      <c r="P55" s="1">
+      <c r="Q55" s="8">
+        <v>24139</v>
+      </c>
+      <c r="R55" s="1">
         <v>50</v>
       </c>
-      <c r="Q55" s="1">
+      <c r="S55" s="1">
         <v>41</v>
       </c>
-      <c r="R55" s="2">
+      <c r="T55" s="2">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="56" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U55" s="2">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="56" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -2033,17 +4020,23 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
-      <c r="P56" s="1">
+      <c r="Q56" s="8">
+        <v>24167</v>
+      </c>
+      <c r="R56" s="1">
         <v>51</v>
       </c>
-      <c r="Q56" s="1">
+      <c r="S56" s="1">
         <v>42</v>
       </c>
-      <c r="R56" s="2">
+      <c r="T56" s="2">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="57" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U56" s="2">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="57" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -2053,17 +4046,23 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
-      <c r="P57" s="1">
+      <c r="Q57" s="8">
+        <v>24198</v>
+      </c>
+      <c r="R57" s="1">
         <v>52</v>
       </c>
-      <c r="Q57" s="1">
+      <c r="S57" s="1">
         <v>43</v>
       </c>
-      <c r="R57" s="2">
+      <c r="T57" s="2">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="58" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U57" s="2">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="58" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -2073,17 +4072,23 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
-      <c r="P58" s="1">
+      <c r="Q58" s="8">
+        <v>24228</v>
+      </c>
+      <c r="R58" s="1">
         <v>53</v>
       </c>
-      <c r="Q58" s="1">
+      <c r="S58" s="1">
         <v>44</v>
       </c>
-      <c r="R58" s="2">
+      <c r="T58" s="2">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="59" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U58" s="2">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="59" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -2093,17 +4098,23 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
-      <c r="P59" s="1">
+      <c r="Q59" s="8">
+        <v>24259</v>
+      </c>
+      <c r="R59" s="1">
         <v>54</v>
       </c>
-      <c r="Q59" s="1">
+      <c r="S59" s="1">
         <v>45</v>
       </c>
-      <c r="R59" s="2">
+      <c r="T59" s="2">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="60" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U59" s="2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="60" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -2113,17 +4124,23 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
-      <c r="P60" s="1">
+      <c r="Q60" s="8">
+        <v>24289</v>
+      </c>
+      <c r="R60" s="1">
         <v>55</v>
       </c>
-      <c r="Q60" s="1">
+      <c r="S60" s="1">
         <v>46</v>
       </c>
-      <c r="R60" s="2">
+      <c r="T60" s="2">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="61" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U60" s="2">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="61" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -2133,17 +4150,23 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
-      <c r="P61" s="1">
+      <c r="Q61" s="8">
+        <v>24320</v>
+      </c>
+      <c r="R61" s="1">
         <v>56</v>
       </c>
-      <c r="Q61" s="1">
+      <c r="S61" s="1">
         <v>47</v>
       </c>
-      <c r="R61" s="2">
+      <c r="T61" s="2">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="62" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U61" s="2">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="62" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -2153,17 +4176,23 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
-      <c r="P62" s="1">
+      <c r="Q62" s="8">
+        <v>24351</v>
+      </c>
+      <c r="R62" s="1">
         <v>57</v>
       </c>
-      <c r="Q62" s="1">
+      <c r="S62" s="1">
         <v>48</v>
       </c>
-      <c r="R62" s="2">
+      <c r="T62" s="2">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="63" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U62" s="2">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="63" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -2173,17 +4202,23 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
-      <c r="P63" s="1">
+      <c r="Q63" s="8">
+        <v>24381</v>
+      </c>
+      <c r="R63" s="1">
         <v>58</v>
       </c>
-      <c r="Q63" s="1">
+      <c r="S63" s="1">
         <v>49</v>
       </c>
-      <c r="R63" s="2">
+      <c r="T63" s="2">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="64" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="U63" s="2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="64" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -2193,17 +4228,23 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
-      <c r="P64" s="1">
+      <c r="Q64" s="8">
+        <v>24412</v>
+      </c>
+      <c r="R64" s="1">
         <v>59</v>
       </c>
-      <c r="Q64" s="1">
+      <c r="S64" s="1">
         <v>50</v>
       </c>
-      <c r="R64" s="2">
+      <c r="T64" s="2">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="65" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U64" s="2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="65" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -2213,17 +4254,23 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
-      <c r="P65" s="1">
+      <c r="Q65" s="8">
+        <v>24442</v>
+      </c>
+      <c r="R65" s="1">
         <v>60</v>
       </c>
-      <c r="Q65" s="1">
+      <c r="S65" s="1">
         <v>51</v>
       </c>
-      <c r="R65" s="2">
+      <c r="T65" s="2">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="66" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U65" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="66" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2233,17 +4280,23 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="P66" s="1">
+      <c r="Q66" s="8">
+        <v>24473</v>
+      </c>
+      <c r="R66" s="1">
         <v>61</v>
       </c>
-      <c r="Q66" s="1">
+      <c r="S66" s="1">
         <v>52</v>
       </c>
-      <c r="R66" s="2">
+      <c r="T66" s="2">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="67" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U66" s="2">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="67" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2253,17 +4306,23 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="P67" s="1">
+      <c r="Q67" s="8">
+        <v>24504</v>
+      </c>
+      <c r="R67" s="1">
         <v>62</v>
       </c>
-      <c r="Q67" s="1">
+      <c r="S67" s="1">
         <v>53</v>
       </c>
-      <c r="R67" s="2">
+      <c r="T67" s="2">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="68" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U67" s="2">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="68" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -2273,17 +4332,23 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
-      <c r="P68" s="1">
+      <c r="Q68" s="8">
+        <v>24532</v>
+      </c>
+      <c r="R68" s="1">
         <v>63</v>
       </c>
-      <c r="Q68" s="1">
+      <c r="S68" s="1">
         <v>54</v>
       </c>
-      <c r="R68" s="2">
+      <c r="T68" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U68" s="2">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="69" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -2293,17 +4358,23 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
-      <c r="P69" s="1">
+      <c r="Q69" s="8">
+        <v>24563</v>
+      </c>
+      <c r="R69" s="1">
         <v>64</v>
       </c>
-      <c r="Q69" s="1">
+      <c r="S69" s="1">
         <v>55</v>
       </c>
-      <c r="R69" s="2">
+      <c r="T69" s="2">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="70" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U69" s="2">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="70" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -2313,17 +4384,23 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
-      <c r="P70" s="1">
+      <c r="Q70" s="8">
+        <v>24593</v>
+      </c>
+      <c r="R70" s="1">
         <v>65</v>
       </c>
-      <c r="Q70" s="1">
+      <c r="S70" s="1">
         <v>56</v>
       </c>
-      <c r="R70" s="2">
+      <c r="T70" s="2">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="71" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U70" s="2">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="71" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -2333,17 +4410,23 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
       <c r="M71" s="3"/>
-      <c r="P71" s="1">
+      <c r="Q71" s="8">
+        <v>24624</v>
+      </c>
+      <c r="R71" s="1">
         <v>66</v>
       </c>
-      <c r="Q71" s="1">
+      <c r="S71" s="1">
         <v>57</v>
       </c>
-      <c r="R71" s="2">
+      <c r="T71" s="2">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="72" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U71" s="2">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="72" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -2353,17 +4436,23 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
-      <c r="P72" s="1">
+      <c r="Q72" s="8">
+        <v>24654</v>
+      </c>
+      <c r="R72" s="1">
         <v>67</v>
       </c>
-      <c r="Q72" s="1">
+      <c r="S72" s="1">
         <v>58</v>
       </c>
-      <c r="R72" s="2">
+      <c r="T72" s="2">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="73" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U72" s="2">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="73" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -2373,17 +4462,23 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
-      <c r="P73" s="1">
+      <c r="Q73" s="8">
+        <v>24685</v>
+      </c>
+      <c r="R73" s="1">
         <v>68</v>
       </c>
-      <c r="Q73" s="1">
+      <c r="S73" s="1">
         <v>59</v>
       </c>
-      <c r="R73" s="2">
+      <c r="T73" s="2">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="74" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U73" s="2">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="74" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -2393,17 +4488,23 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
       <c r="M74" s="3"/>
-      <c r="P74" s="1">
+      <c r="Q74" s="8">
+        <v>24716</v>
+      </c>
+      <c r="R74" s="1">
         <v>69</v>
       </c>
-      <c r="Q74" s="1">
+      <c r="S74" s="1">
         <v>60</v>
       </c>
-      <c r="R74" s="2">
+      <c r="T74" s="2">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="75" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U74" s="2">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="75" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -2413,17 +4514,23 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
-      <c r="P75" s="1">
+      <c r="Q75" s="8">
+        <v>24746</v>
+      </c>
+      <c r="R75" s="1">
         <v>70</v>
       </c>
-      <c r="Q75" s="1">
+      <c r="S75" s="1">
         <v>61</v>
       </c>
-      <c r="R75" s="2">
+      <c r="T75" s="2">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="76" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U75" s="2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="76" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -2433,17 +4540,23 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
-      <c r="P76" s="1">
+      <c r="Q76" s="8">
+        <v>24777</v>
+      </c>
+      <c r="R76" s="1">
         <v>71</v>
       </c>
-      <c r="Q76" s="1">
+      <c r="S76" s="1">
         <v>62</v>
       </c>
-      <c r="R76" s="2">
+      <c r="T76" s="2">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="77" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U76" s="2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="77" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -2453,17 +4566,23 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
       <c r="M77" s="3"/>
-      <c r="P77" s="1">
+      <c r="Q77" s="8">
+        <v>24807</v>
+      </c>
+      <c r="R77" s="1">
         <v>72</v>
       </c>
-      <c r="Q77" s="1">
+      <c r="S77" s="1">
         <v>63</v>
       </c>
-      <c r="R77" s="2">
+      <c r="T77" s="2">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="78" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U77" s="2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -2473,8 +4592,9 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
-    </row>
-    <row r="79" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q78" s="2"/>
+    </row>
+    <row r="79" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -2489,8 +4609,10 @@
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
-    </row>
-    <row r="80" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q79" s="2"/>
+      <c r="R79" s="2"/>
+    </row>
+    <row r="80" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C80" s="2"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -2505,8 +4627,10 @@
       <c r="N80" s="3"/>
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
-    </row>
-    <row r="81" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="Q80" s="2"/>
+      <c r="R80" s="2"/>
+    </row>
+    <row r="81" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -2521,8 +4645,10 @@
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
-    </row>
-    <row r="82" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="Q81" s="2"/>
+      <c r="R81" s="2"/>
+    </row>
+    <row r="82" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -2537,6 +4663,7 @@
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
       <c r="P82" s="2"/>
+      <c r="R82" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2546,5 +4673,6 @@
   <ignoredErrors>
     <ignoredError sqref="D13:N37" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>